<commit_message>
Update LC & RLC Formula
Update Spreadsheets
</commit_message>
<xml_diff>
--- a/Series LC & RLC Circuit Designs.xlsx
+++ b/Series LC & RLC Circuit Designs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
   <si>
     <t xml:space="preserve">Coil Design</t>
   </si>
@@ -100,7 +100,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> ( </t>
+      <t xml:space="preserve"> (</t>
     </r>
     <r>
       <rPr>
@@ -117,14 +117,55 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> )</t>
+      <t xml:space="preserve">) </t>
     </r>
   </si>
   <si>
     <t xml:space="preserve"> m²</t>
   </si>
   <si>
+    <t xml:space="preserve">Example:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inductance of a Coil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A battery with a 9 Volt, 100mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V =</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Volts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A =</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Mili Ampere</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (mA)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -227,6 +268,24 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">A = 100 mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Amps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
     <t xml:space="preserve">L = </t>
   </si>
   <si>
@@ -270,13 +329,16 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve"> Ohms</t>
+  </si>
+  <si>
     <t xml:space="preserve">Series LC &amp; RLC Circuit Design</t>
   </si>
   <si>
     <t xml:space="preserve">Finding Capasitor Value in LC Circuit</t>
   </si>
   <si>
-    <t xml:space="preserve">Finding Resistor Value for LRC Circuit</t>
+    <t xml:space="preserve">Finding Resistor Value in LRC Circuit</t>
   </si>
   <si>
     <t xml:space="preserve">Resonant Frequency of LC Circuits</t>
@@ -337,20 +399,47 @@
   <si>
     <r>
       <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">XL = </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2πfL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <u val="single"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Circuit Impedance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ( </t>
+      <t xml:space="preserve">Capacitive Reactance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
     </r>
     <r>
       <rPr>
@@ -359,24 +448,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Z </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">XC) </t>
     </r>
     <r>
       <rPr>
@@ -386,94 +458,6 @@
       </rPr>
       <t xml:space="preserve">:</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">XL = </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">2πfL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ohms</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Z = </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">√R²+(XL-XC)²</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Capacitive Reactance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">XC) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Z =</t>
   </si>
   <si>
     <r>
@@ -574,6 +558,185 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">Resistor Value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ( </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ) :</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">R = </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">XL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">–</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">XC =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Circuit Impedance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ( </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Z </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency ( F ) = </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Hertz </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Hz)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Z = </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">√R²+(XL-XC)²</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Z =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C = (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">)² ꞉ L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2πF</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">Quality Factor</t>
     </r>
     <r>
@@ -603,22 +766,20 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Resistor Value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ( </t>
+    <t xml:space="preserve">Q = XL/R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C = </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Farad </t>
     </r>
     <r>
       <rPr>
@@ -627,28 +788,26 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">R</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ) :</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Q = XL/R</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">R = </t>
+      <t xml:space="preserve">(F)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> MicroFarad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
     </r>
     <r>
       <rPr>
@@ -657,157 +816,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">XL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">–</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">XC =</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Circuit Current</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ( </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">I</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ) :</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">I = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frequency ( F ) = </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Hertz </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Hz)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> = </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Amps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C = (</t>
-  </si>
-  <si>
-    <t xml:space="preserve">)² ꞉ L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2πF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C = </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Farad </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(F)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> MicroFarad</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve">µF</t>
     </r>
     <r>
@@ -818,6 +826,9 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Q Factor = </t>
   </si>
 </sst>
 </file>
@@ -828,7 +839,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -852,8 +863,8 @@
     <font>
       <b val="true"/>
       <sz val="20"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Andale Mono"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="15"/>
@@ -869,6 +880,18 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF999999"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -906,8 +929,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF1A237E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -944,14 +974,8 @@
         <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF999999"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="18">
+  <borders count="16">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1064,20 +1088,6 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right/>
-      <top style="hair"/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1104,7 +1114,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="72">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1181,14 +1191,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1205,7 +1219,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1221,75 +1235,119 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1297,11 +1355,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1309,64 +1379,28 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1428,7 +1462,7 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF999999"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF1A237E"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -1446,19 +1480,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>673560</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:colOff>211680</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>149760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>633240</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>79560</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>419040</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Image 1" descr=""/>
+        <xdr:cNvPr id="0" name="Image 2" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1467,8 +1501,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2298960" y="3757680"/>
-          <a:ext cx="1585440" cy="621360"/>
+          <a:off x="1839600" y="7798680"/>
+          <a:ext cx="2649600" cy="1349280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1482,20 +1516,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>199440</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1440</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>407160</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>27360</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>756000</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Image 2" descr=""/>
+        <xdr:cNvPr id="1" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1504,8 +1538,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1824840" y="7764480"/>
-          <a:ext cx="2646000" cy="1349640"/>
+          <a:off x="2443320" y="3783960"/>
+          <a:ext cx="1568880" cy="622440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1525,10 +1559,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:Q74"/>
+  <dimension ref="B3:X77"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J70" activeCellId="0" sqref="J70"/>
+      <selection pane="topLeft" activeCell="F90" activeCellId="0" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1642,7 +1676,7 @@
       <c r="M10" s="17"/>
       <c r="N10" s="16"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="14"/>
       <c r="C11" s="18" t="s">
         <v>4</v>
@@ -1664,49 +1698,49 @@
       <c r="K11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="L11" s="7"/>
+      <c r="L11" s="21"/>
       <c r="M11" s="17"/>
       <c r="N11" s="16"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="14"/>
-      <c r="C12" s="21" t="n">
+      <c r="C12" s="22" t="n">
         <v>30</v>
       </c>
-      <c r="D12" s="22" t="n">
+      <c r="D12" s="23" t="n">
         <v>0.5</v>
       </c>
-      <c r="E12" s="23" t="n">
-        <v>100</v>
-      </c>
-      <c r="F12" s="24" t="n">
+      <c r="E12" s="24" t="n">
+        <v>50</v>
+      </c>
+      <c r="F12" s="25" t="n">
         <f aca="false">D12*E12</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="G12" s="16"/>
       <c r="I12" s="14"/>
       <c r="J12" s="19"/>
-      <c r="K12" s="25" t="s">
+      <c r="K12" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="L12" s="7"/>
+      <c r="L12" s="21"/>
       <c r="M12" s="17"/>
       <c r="N12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="14"/>
-      <c r="C13" s="26" t="n">
+      <c r="C13" s="27" t="n">
         <f aca="false">C12*(10^(-3))</f>
         <v>0.03</v>
       </c>
-      <c r="D13" s="26" t="n">
+      <c r="D13" s="27" t="n">
         <f aca="false">D12*(10^(-3))</f>
         <v>0.0005</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="24" t="n">
+      <c r="E13" s="28"/>
+      <c r="F13" s="25" t="n">
         <f aca="false">F12*(10^(-3))</f>
-        <v>0.05</v>
+        <v>0.025</v>
       </c>
       <c r="G13" s="16"/>
       <c r="I13" s="14"/>
@@ -1718,10 +1752,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="14"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
       <c r="G14" s="16"/>
       <c r="I14" s="14"/>
       <c r="J14" s="17"/>
@@ -1733,7 +1767,7 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="14"/>
       <c r="C15" s="17"/>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="30" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="17"/>
@@ -1749,19 +1783,19 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="14"/>
       <c r="C16" s="17"/>
-      <c r="D16" s="29"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="16"/>
       <c r="I16" s="14"/>
-      <c r="J16" s="30" t="s">
+      <c r="J16" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="K16" s="31" t="n">
+      <c r="K16" s="32" t="n">
         <f aca="false">D35/(E18/D13)</f>
-        <v>100</v>
-      </c>
-      <c r="L16" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="33" t="s">
         <v>12</v>
       </c>
       <c r="M16" s="17"/>
@@ -1775,23 +1809,23 @@
       <c r="F17" s="17"/>
       <c r="G17" s="16"/>
       <c r="I17" s="14"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
       <c r="M17" s="17"/>
       <c r="N17" s="16"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="14"/>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="34" t="n">
+      <c r="D18" s="34"/>
+      <c r="E18" s="35" t="n">
         <f aca="false">3.14 * (C13^(2))</f>
         <v>0.002826</v>
       </c>
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="36" t="s">
         <v>14</v>
       </c>
       <c r="G18" s="16"/>
@@ -1803,18 +1837,18 @@
       <c r="N18" s="16"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="38"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="38"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="39"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="39"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="14"/>
@@ -1823,6 +1857,12 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="16"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="14"/>
@@ -1831,16 +1871,32 @@
       <c r="E21" s="2"/>
       <c r="F21" s="4"/>
       <c r="G21" s="16"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="16"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="14"/>
-      <c r="C22" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
+      <c r="C22" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
       <c r="G22" s="16"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="16"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="14"/>
@@ -1849,6 +1905,14 @@
       <c r="E23" s="6"/>
       <c r="F23" s="7"/>
       <c r="G23" s="16"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="16"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="14"/>
@@ -1857,14 +1921,35 @@
       <c r="E24" s="6"/>
       <c r="F24" s="7"/>
       <c r="G24" s="16"/>
+      <c r="I24" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="17"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="16"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="14"/>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="40"/>
+      <c r="F25" s="43"/>
       <c r="G25" s="16"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" s="45" t="n">
+        <f aca="false">9</f>
+        <v>9</v>
+      </c>
+      <c r="L25" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="M25" s="17"/>
+      <c r="N25" s="16"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="14"/>
@@ -1873,64 +1958,138 @@
       <c r="E26" s="6"/>
       <c r="F26" s="7"/>
       <c r="G26" s="16"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" s="45" t="n">
+        <f aca="false">100</f>
+        <v>100</v>
+      </c>
+      <c r="L26" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="M26" s="17"/>
+      <c r="N26" s="16"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="14"/>
-      <c r="C27" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
+      <c r="C27" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
       <c r="G27" s="16"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="16"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="14"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
       <c r="G28" s="16"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="L28" s="49" t="n">
+        <v>100</v>
+      </c>
+      <c r="M28" s="17"/>
+      <c r="N28" s="16"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="14"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
       <c r="G29" s="16"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="50" t="n">
+        <v>1000</v>
+      </c>
+      <c r="M29" s="17"/>
+      <c r="N29" s="16"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="14"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
       <c r="G30" s="16"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="16"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="14"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="16"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="L31" s="52" t="n">
+        <f aca="false">100/1000</f>
+        <v>0.1</v>
+      </c>
+      <c r="M31" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="N31" s="16"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="14"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
       <c r="G32" s="16"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="42"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="16"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="14"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
       <c r="G33" s="16"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="16"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="14"/>
@@ -1939,48 +2098,81 @@
       <c r="E34" s="17"/>
       <c r="F34" s="17"/>
       <c r="G34" s="16"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="54"/>
+      <c r="K34" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="L34" s="29"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="16"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="14"/>
-      <c r="C35" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="43" t="n">
-        <f aca="false">1*((E12^(2)*E18)/F13)</f>
-        <v>565.2</v>
-      </c>
-      <c r="E35" s="44" t="s">
-        <v>18</v>
+      <c r="C35" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="52" t="n">
+        <f aca="false">ROUND(1*((E12^(2)*E18)/F13),2)</f>
+        <v>282.6</v>
+      </c>
+      <c r="E35" s="53" t="s">
+        <v>32</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="16"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="42"/>
+      <c r="K35" s="42"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="14"/>
       <c r="C36" s="17"/>
-      <c r="D36" s="45" t="n">
-        <f aca="false"> D35*(1.26*10^(-6))</f>
-        <v>0.000712152</v>
-      </c>
-      <c r="E36" s="44" t="s">
-        <v>19</v>
+      <c r="D36" s="52" t="n">
+        <f aca="false">D35*(1.26*10^(-6))</f>
+        <v>0.000356076</v>
+      </c>
+      <c r="E36" s="53" t="s">
+        <v>33</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="16"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="K36" s="52" t="n">
+        <f aca="false">K25/L31</f>
+        <v>90</v>
+      </c>
+      <c r="L36" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="M36" s="29"/>
+      <c r="N36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="36"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="38"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="39"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="38"/>
+      <c r="M37" s="38"/>
+      <c r="N37" s="39"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="1"/>
       <c r="C40" s="2"/>
       <c r="D40" s="3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -2035,31 +2227,31 @@
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
       <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
-      <c r="O44" s="12"/>
-      <c r="P44" s="12"/>
-      <c r="Q44" s="13"/>
+      <c r="N44" s="13"/>
+      <c r="S44" s="12"/>
+      <c r="T44" s="12"/>
+      <c r="U44" s="12"/>
+      <c r="V44" s="12"/>
+      <c r="W44" s="12"/>
+      <c r="X44" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="14"/>
       <c r="C45" s="15" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
       <c r="F45" s="15"/>
       <c r="G45" s="16"/>
       <c r="I45" s="14"/>
-      <c r="J45" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="K45" s="46"/>
-      <c r="L45" s="46"/>
-      <c r="M45" s="46"/>
-      <c r="N45" s="28"/>
-      <c r="O45" s="28"/>
-      <c r="P45" s="28"/>
-      <c r="Q45" s="16"/>
+      <c r="J45" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="K45" s="58"/>
+      <c r="L45" s="58"/>
+      <c r="M45" s="58"/>
+      <c r="N45" s="16"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="14"/>
@@ -2073,10 +2265,7 @@
       <c r="K46" s="17"/>
       <c r="L46" s="17"/>
       <c r="M46" s="17"/>
-      <c r="N46" s="28"/>
-      <c r="O46" s="28"/>
-      <c r="P46" s="28"/>
-      <c r="Q46" s="16"/>
+      <c r="N46" s="16"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="14"/>
@@ -2086,37 +2275,29 @@
       <c r="F47" s="13"/>
       <c r="G47" s="16"/>
       <c r="I47" s="14"/>
-      <c r="J47" s="28"/>
-      <c r="K47" s="28"/>
-      <c r="L47" s="28"/>
-      <c r="M47" s="28"/>
-      <c r="N47" s="28"/>
-      <c r="O47" s="28"/>
-      <c r="P47" s="28"/>
-      <c r="Q47" s="16"/>
+      <c r="J47" s="29"/>
+      <c r="K47" s="29"/>
+      <c r="L47" s="29"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="16"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="14"/>
-      <c r="C48" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
+      <c r="C48" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" s="59"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
       <c r="G48" s="16"/>
       <c r="I48" s="14"/>
-      <c r="J48" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="K48" s="28"/>
-      <c r="L48" s="28"/>
-      <c r="M48" s="28"/>
-      <c r="N48" s="28"/>
-      <c r="O48" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="P48" s="28"/>
-      <c r="Q48" s="16"/>
+      <c r="J48" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="K48" s="29"/>
+      <c r="L48" s="29"/>
+      <c r="M48" s="29"/>
+      <c r="N48" s="16"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="14"/>
@@ -2126,14 +2307,11 @@
       <c r="F49" s="16"/>
       <c r="G49" s="16"/>
       <c r="I49" s="14"/>
-      <c r="J49" s="28"/>
-      <c r="K49" s="28"/>
-      <c r="L49" s="28"/>
-      <c r="M49" s="16"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="28"/>
-      <c r="P49" s="28"/>
-      <c r="Q49" s="16"/>
+      <c r="J49" s="29"/>
+      <c r="K49" s="29"/>
+      <c r="L49" s="29"/>
+      <c r="M49" s="29"/>
+      <c r="N49" s="16"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="14"/>
@@ -2143,23 +2321,18 @@
       <c r="F50" s="16"/>
       <c r="G50" s="16"/>
       <c r="I50" s="14"/>
-      <c r="J50" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="K50" s="24" t="n">
-        <f aca="false"> ROUND((2*3.14) * D64 * D35,2)</f>
-        <v>2825366.98</v>
-      </c>
-      <c r="L50" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="M50" s="16"/>
-      <c r="N50" s="14"/>
-      <c r="O50" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="P50" s="28"/>
-      <c r="Q50" s="16"/>
+      <c r="J50" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="K50" s="25" t="n">
+        <f aca="false">ROUND((2*3.14) * D64 * D35,2)</f>
+        <v>106483.68</v>
+      </c>
+      <c r="L50" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="M50" s="29"/>
+      <c r="N50" s="16"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="14"/>
@@ -2169,14 +2342,11 @@
       <c r="F51" s="16"/>
       <c r="G51" s="16"/>
       <c r="I51" s="14"/>
-      <c r="J51" s="28"/>
-      <c r="K51" s="28"/>
-      <c r="L51" s="28"/>
-      <c r="M51" s="16"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="28"/>
-      <c r="P51" s="28"/>
-      <c r="Q51" s="16"/>
+      <c r="J51" s="29"/>
+      <c r="K51" s="29"/>
+      <c r="L51" s="29"/>
+      <c r="M51" s="29"/>
+      <c r="N51" s="16"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="14"/>
@@ -2186,203 +2356,157 @@
       <c r="F52" s="16"/>
       <c r="G52" s="16"/>
       <c r="I52" s="14"/>
-      <c r="J52" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="K52" s="28"/>
-      <c r="L52" s="28"/>
-      <c r="M52" s="16"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="P52" s="24" t="n">
-        <f aca="false">ROUND(SQRT(K58^(2) + (K50 - K54)^(2)), 2)</f>
-        <v>3995672.3</v>
-      </c>
-      <c r="Q52" s="51" t="s">
-        <v>27</v>
-      </c>
+      <c r="J52" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="K52" s="29"/>
+      <c r="L52" s="29"/>
+      <c r="M52" s="29"/>
+      <c r="N52" s="16"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="14"/>
-      <c r="C53" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="D53" s="52"/>
-      <c r="E53" s="52"/>
-      <c r="F53" s="52"/>
+      <c r="C53" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" s="61"/>
+      <c r="E53" s="61"/>
+      <c r="F53" s="61"/>
       <c r="G53" s="16"/>
       <c r="I53" s="14"/>
-      <c r="J53" s="28"/>
-      <c r="K53" s="28"/>
-      <c r="L53" s="28"/>
-      <c r="M53" s="16"/>
-      <c r="N53" s="14"/>
-      <c r="O53" s="28"/>
-      <c r="P53" s="28"/>
-      <c r="Q53" s="16"/>
+      <c r="J53" s="29"/>
+      <c r="K53" s="29"/>
+      <c r="L53" s="29"/>
+      <c r="M53" s="29"/>
+      <c r="N53" s="16"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="14"/>
-      <c r="C54" s="52"/>
-      <c r="D54" s="52"/>
-      <c r="E54" s="52"/>
-      <c r="F54" s="52"/>
+      <c r="C54" s="61"/>
+      <c r="D54" s="61"/>
+      <c r="E54" s="61"/>
+      <c r="F54" s="61"/>
       <c r="G54" s="16"/>
       <c r="I54" s="14"/>
-      <c r="J54" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="K54" s="24" t="n">
-        <f aca="false"> (2*3.14) * D64 * D70</f>
-        <v>3.53936323491593E-007</v>
-      </c>
-      <c r="L54" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="M54" s="16"/>
-      <c r="N54" s="14"/>
-      <c r="O54" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="P54" s="28"/>
-      <c r="Q54" s="16"/>
+      <c r="J54" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="K54" s="25" t="n">
+        <f aca="false">(2*3.14) * D64 * D72</f>
+        <v>9.39111044997693E-006</v>
+      </c>
+      <c r="L54" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="M54" s="29"/>
+      <c r="N54" s="16"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="14"/>
-      <c r="C55" s="52"/>
-      <c r="D55" s="52"/>
-      <c r="E55" s="52"/>
-      <c r="F55" s="52"/>
+      <c r="C55" s="61"/>
+      <c r="D55" s="61"/>
+      <c r="E55" s="61"/>
+      <c r="F55" s="61"/>
       <c r="G55" s="16"/>
       <c r="I55" s="14"/>
-      <c r="J55" s="28"/>
-      <c r="K55" s="28"/>
-      <c r="L55" s="28"/>
-      <c r="M55" s="16"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="28"/>
-      <c r="P55" s="28"/>
-      <c r="Q55" s="16"/>
+      <c r="J55" s="29"/>
+      <c r="K55" s="29"/>
+      <c r="L55" s="29"/>
+      <c r="M55" s="29"/>
+      <c r="N55" s="16"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="14"/>
-      <c r="C56" s="52"/>
-      <c r="D56" s="52"/>
-      <c r="E56" s="52"/>
-      <c r="F56" s="52"/>
+      <c r="C56" s="61"/>
+      <c r="D56" s="61"/>
+      <c r="E56" s="61"/>
+      <c r="F56" s="61"/>
       <c r="G56" s="16"/>
       <c r="I56" s="14"/>
-      <c r="J56" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="K56" s="28"/>
-      <c r="L56" s="28"/>
-      <c r="M56" s="16"/>
-      <c r="N56" s="14"/>
-      <c r="O56" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="P56" s="28"/>
-      <c r="Q56" s="16"/>
+      <c r="J56" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="K56" s="29"/>
+      <c r="L56" s="29"/>
+      <c r="M56" s="29"/>
+      <c r="N56" s="16"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="14"/>
-      <c r="C57" s="52"/>
-      <c r="D57" s="52"/>
-      <c r="E57" s="52"/>
-      <c r="F57" s="52"/>
+      <c r="C57" s="61"/>
+      <c r="D57" s="61"/>
+      <c r="E57" s="61"/>
+      <c r="F57" s="61"/>
       <c r="G57" s="16"/>
       <c r="I57" s="14"/>
-      <c r="J57" s="28"/>
-      <c r="K57" s="28"/>
-      <c r="L57" s="28"/>
-      <c r="M57" s="16"/>
-      <c r="N57" s="14"/>
-      <c r="O57" s="53"/>
-      <c r="P57" s="28"/>
-      <c r="Q57" s="51"/>
+      <c r="J57" s="29"/>
+      <c r="K57" s="29"/>
+      <c r="L57" s="29"/>
+      <c r="M57" s="29"/>
+      <c r="N57" s="16"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="14"/>
-      <c r="C58" s="52"/>
-      <c r="D58" s="52"/>
-      <c r="E58" s="52"/>
-      <c r="F58" s="52"/>
+      <c r="C58" s="61"/>
+      <c r="D58" s="61"/>
+      <c r="E58" s="61"/>
+      <c r="F58" s="61"/>
       <c r="G58" s="16"/>
       <c r="I58" s="14"/>
-      <c r="J58" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="K58" s="34" t="n">
-        <f aca="false"> ROUND(K50 - K54, 2)</f>
-        <v>2825366.98</v>
-      </c>
-      <c r="L58" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="M58" s="16"/>
-      <c r="N58" s="14"/>
-      <c r="O58" s="28"/>
-      <c r="P58" s="28"/>
-      <c r="Q58" s="16"/>
+      <c r="J58" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="K58" s="25" t="n">
+        <f aca="false">ROUND(K50 - K54, 2)</f>
+        <v>106483.68</v>
+      </c>
+      <c r="L58" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="M58" s="29"/>
+      <c r="N58" s="16"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="14"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="52"/>
-      <c r="E59" s="52"/>
-      <c r="F59" s="52"/>
+      <c r="C59" s="61"/>
+      <c r="D59" s="61"/>
+      <c r="E59" s="61"/>
+      <c r="F59" s="61"/>
       <c r="G59" s="16"/>
       <c r="I59" s="14"/>
-      <c r="J59" s="28"/>
-      <c r="K59" s="28"/>
-      <c r="L59" s="28"/>
-      <c r="M59" s="16"/>
-      <c r="N59" s="28"/>
-      <c r="O59" s="34" t="n">
-        <f aca="false"> ROUND(K50/K58,2)</f>
-        <v>1</v>
-      </c>
-      <c r="P59" s="28"/>
-      <c r="Q59" s="16"/>
+      <c r="J59" s="29"/>
+      <c r="K59" s="29"/>
+      <c r="L59" s="29"/>
+      <c r="M59" s="29"/>
+      <c r="N59" s="16"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="14"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
       <c r="G60" s="16"/>
       <c r="I60" s="14"/>
-      <c r="J60" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="K60" s="28"/>
-      <c r="L60" s="28"/>
-      <c r="M60" s="16"/>
-      <c r="N60" s="28"/>
-      <c r="O60" s="28"/>
-      <c r="P60" s="28"/>
-      <c r="Q60" s="16"/>
+      <c r="J60" s="29"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="29"/>
+      <c r="M60" s="29"/>
+      <c r="N60" s="16"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="36"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="38"/>
-      <c r="I61" s="14"/>
-      <c r="J61" s="28"/>
-      <c r="K61" s="28"/>
-      <c r="L61" s="28"/>
-      <c r="M61" s="16"/>
-      <c r="N61" s="28"/>
-      <c r="O61" s="28"/>
-      <c r="P61" s="28"/>
-      <c r="Q61" s="16"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="39"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="38"/>
+      <c r="K61" s="38"/>
+      <c r="L61" s="38"/>
+      <c r="M61" s="38"/>
+      <c r="N61" s="39"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="11"/>
@@ -2391,207 +2515,256 @@
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
       <c r="G62" s="13"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="K62" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="L62" s="57"/>
-      <c r="M62" s="16"/>
-      <c r="N62" s="28"/>
-      <c r="O62" s="28"/>
-      <c r="P62" s="28"/>
-      <c r="Q62" s="16"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
+      <c r="M62" s="12"/>
+      <c r="N62" s="13"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="14"/>
-      <c r="C63" s="28"/>
-      <c r="D63" s="28"/>
-      <c r="E63" s="28"/>
-      <c r="F63" s="28"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="29"/>
       <c r="G63" s="16"/>
       <c r="I63" s="14"/>
-      <c r="J63" s="55"/>
-      <c r="K63" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="L63" s="59"/>
-      <c r="M63" s="16"/>
-      <c r="N63" s="28"/>
-      <c r="O63" s="28"/>
-      <c r="P63" s="28"/>
-      <c r="Q63" s="16"/>
+      <c r="J63" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="K63" s="29"/>
+      <c r="L63" s="29"/>
+      <c r="M63" s="29"/>
+      <c r="N63" s="16"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="14"/>
-      <c r="C64" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="D64" s="31" t="n">
-        <v>796</v>
-      </c>
-      <c r="E64" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="F64" s="28"/>
+      <c r="C64" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="D64" s="32" t="n">
+        <v>60</v>
+      </c>
+      <c r="E64" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="F64" s="29"/>
       <c r="G64" s="16"/>
       <c r="I64" s="14"/>
-      <c r="J64" s="28"/>
-      <c r="K64" s="28"/>
-      <c r="L64" s="28"/>
-      <c r="M64" s="16"/>
-      <c r="N64" s="28"/>
-      <c r="O64" s="28"/>
-      <c r="P64" s="28"/>
-      <c r="Q64" s="16"/>
+      <c r="J64" s="29"/>
+      <c r="K64" s="29"/>
+      <c r="L64" s="29"/>
+      <c r="M64" s="29"/>
+      <c r="N64" s="16"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="14"/>
-      <c r="C65" s="28"/>
-      <c r="D65" s="31"/>
-      <c r="E65" s="31"/>
-      <c r="F65" s="28"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="29"/>
       <c r="G65" s="16"/>
       <c r="I65" s="14"/>
-      <c r="J65" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="K65" s="63" t="n">
-        <f aca="false"> 1/P52</f>
-        <v>2.50270774207384E-007</v>
-      </c>
-      <c r="L65" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="M65" s="16"/>
-      <c r="N65" s="28"/>
-      <c r="O65" s="28"/>
-      <c r="P65" s="28"/>
-      <c r="Q65" s="16"/>
+      <c r="J65" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="K65" s="29"/>
+      <c r="L65" s="29"/>
+      <c r="M65" s="29"/>
+      <c r="N65" s="16"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="14"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="28"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
       <c r="G66" s="16"/>
       <c r="I66" s="14"/>
-      <c r="J66" s="62"/>
-      <c r="K66" s="62"/>
-      <c r="L66" s="62"/>
-      <c r="M66" s="28"/>
-      <c r="N66" s="28"/>
-      <c r="O66" s="28"/>
-      <c r="P66" s="28"/>
-      <c r="Q66" s="16"/>
+      <c r="J66" s="29"/>
+      <c r="K66" s="29"/>
+      <c r="L66" s="29"/>
+      <c r="M66" s="29"/>
+      <c r="N66" s="16"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="14"/>
-      <c r="C67" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="D67" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="E67" s="65" t="s">
-        <v>46</v>
-      </c>
-      <c r="F67" s="28"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="29"/>
       <c r="G67" s="16"/>
       <c r="I67" s="14"/>
-      <c r="J67" s="28"/>
-      <c r="K67" s="28"/>
-      <c r="L67" s="28"/>
-      <c r="M67" s="28"/>
-      <c r="N67" s="28"/>
-      <c r="O67" s="28"/>
-      <c r="P67" s="28"/>
-      <c r="Q67" s="16"/>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J67" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="K67" s="25" t="n">
+        <f aca="false">ROUND(SQRT(F73^(2) + (F65 - F69)^(2)), 2)</f>
+        <v>0</v>
+      </c>
+      <c r="L67" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="M67" s="29"/>
+      <c r="N67" s="16"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="14"/>
-      <c r="C68" s="55"/>
-      <c r="D68" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="E68" s="65"/>
-      <c r="F68" s="28"/>
+      <c r="C68" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D68" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" s="66" t="s">
+        <v>52</v>
+      </c>
+      <c r="F68" s="29"/>
       <c r="G68" s="16"/>
-      <c r="I68" s="36"/>
-      <c r="J68" s="37"/>
-      <c r="K68" s="37"/>
-      <c r="L68" s="37"/>
-      <c r="M68" s="37"/>
-      <c r="N68" s="37"/>
-      <c r="O68" s="37"/>
-      <c r="P68" s="37"/>
-      <c r="Q68" s="38"/>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I68" s="14"/>
+      <c r="J68" s="29"/>
+      <c r="K68" s="29"/>
+      <c r="L68" s="29"/>
+      <c r="M68" s="29"/>
+      <c r="N68" s="16"/>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="14"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E69" s="66"/>
+      <c r="F69" s="29"/>
       <c r="G69" s="16"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="K69" s="29"/>
+      <c r="L69" s="29"/>
+      <c r="M69" s="29"/>
+      <c r="N69" s="16"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="14"/>
-      <c r="C70" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="D70" s="24" t="n">
-        <f aca="false">(1/(2*(3.14)*D64))^(2)/D35</f>
-        <v>7.08031245982286E-011</v>
-      </c>
-      <c r="E70" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="F70" s="28"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="29"/>
       <c r="G70" s="16"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="29"/>
+      <c r="K70" s="29"/>
+      <c r="L70" s="29"/>
+      <c r="M70" s="29"/>
+      <c r="N70" s="16"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="14"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="24" t="n">
-        <f aca="false">D70*(10^(6))</f>
-        <v>7.08031245982286E-005</v>
-      </c>
-      <c r="E71" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="F71" s="28"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="29"/>
+      <c r="E71" s="29"/>
+      <c r="F71" s="29"/>
       <c r="G71" s="16"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="67" t="s">
+        <v>55</v>
+      </c>
+      <c r="K71" s="29"/>
+      <c r="L71" s="29"/>
+      <c r="M71" s="29"/>
+      <c r="N71" s="16"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="14"/>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
-      <c r="E72" s="28"/>
-      <c r="F72" s="28"/>
+      <c r="C72" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D72" s="68" t="n">
+        <f aca="false">(1/(2*(3.14)*D64))^(2)/D35</f>
+        <v>2.4923329219684E-008</v>
+      </c>
+      <c r="E72" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="F72" s="29"/>
       <c r="G72" s="16"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="67"/>
+      <c r="K72" s="29"/>
+      <c r="L72" s="57"/>
+      <c r="M72" s="29"/>
+      <c r="N72" s="16"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="14"/>
-      <c r="C73" s="28"/>
-      <c r="D73" s="28"/>
-      <c r="E73" s="28"/>
-      <c r="F73" s="28"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="69" t="n">
+        <f aca="false">ROUND(D72*(10^(6)),3)</f>
+        <v>0.025</v>
+      </c>
+      <c r="E73" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="F73" s="29"/>
       <c r="G73" s="16"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="29"/>
+      <c r="K73" s="29"/>
+      <c r="L73" s="29"/>
+      <c r="M73" s="29"/>
+      <c r="N73" s="16"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="36"/>
-      <c r="C74" s="37"/>
-      <c r="D74" s="37"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="37"/>
-      <c r="G74" s="38"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="39"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="K74" s="70" t="n">
+        <f aca="false">ROUND(K50/K58,2)</f>
+        <v>1</v>
+      </c>
+      <c r="L74" s="71" t="str">
+        <f aca="false">IF(K74&gt;0.5, "Under-damped (Q &gt; 1/2)", IF(K74&lt;0.5, "Over-damped (Q &lt; 1/2)", "Critically damped (Q = 1/2)"))</f>
+        <v>Under-damped (Q &gt; 1/2)</v>
+      </c>
+      <c r="M74" s="71"/>
+      <c r="N74" s="16"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I75" s="14"/>
+      <c r="J75" s="31"/>
+      <c r="K75" s="31"/>
+      <c r="L75" s="31"/>
+      <c r="M75" s="71"/>
+      <c r="N75" s="16"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I76" s="14"/>
+      <c r="J76" s="29"/>
+      <c r="K76" s="29"/>
+      <c r="L76" s="29"/>
+      <c r="M76" s="29"/>
+      <c r="N76" s="16"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I77" s="37"/>
+      <c r="J77" s="38"/>
+      <c r="K77" s="38"/>
+      <c r="L77" s="38"/>
+      <c r="M77" s="38"/>
+      <c r="N77" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="27">
     <mergeCell ref="D3:L5"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="J8:M8"/>
@@ -2603,20 +2776,22 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="C27:F33"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="J33:J34"/>
     <mergeCell ref="D40:L42"/>
     <mergeCell ref="C45:F45"/>
     <mergeCell ref="J45:M45"/>
     <mergeCell ref="C48:F48"/>
     <mergeCell ref="C53:F59"/>
-    <mergeCell ref="O56:O57"/>
-    <mergeCell ref="J62:J63"/>
     <mergeCell ref="D64:D65"/>
     <mergeCell ref="E64:E65"/>
-    <mergeCell ref="J65:J66"/>
-    <mergeCell ref="K65:K66"/>
-    <mergeCell ref="L65:L66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="J71:J72"/>
+    <mergeCell ref="J74:J75"/>
+    <mergeCell ref="K74:K75"/>
+    <mergeCell ref="L74:M75"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>